<commit_message>
updating previously not updated files
</commit_message>
<xml_diff>
--- a/ann_v1_visualization.xlsx
+++ b/ann_v1_visualization.xlsx
@@ -103,13 +103,13 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -140,8 +140,8 @@
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="601640" cy="475002"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2"/>
@@ -177,6 +177,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -234,7 +235,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2"/>
@@ -298,8 +299,8 @@
       <xdr:rowOff>105507</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="509435" cy="320793"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3"/>
@@ -335,6 +336,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -405,7 +407,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3"/>
@@ -723,8 +725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -739,13 +741,13 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="1">
         <v>4</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="1">
         <v>1.0854671899999999</v>
       </c>
       <c r="E2" s="2"/>
@@ -755,37 +757,37 @@
       <c r="I2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="1"/>
+      <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="1">
         <v>5</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="1">
         <v>1.0650397599999999</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="3">
+      <c r="F3" s="1">
         <f>(B2*D2)+(B3*D3)+(B4*D4)</f>
         <v>16.500698010000001</v>
       </c>
       <c r="G3" s="2"/>
-      <c r="H3" s="3">
+      <c r="H3" s="1">
         <v>-12.878135139999999</v>
       </c>
       <c r="I3" s="4"/>
-      <c r="J3" s="3">
+      <c r="J3" s="1">
         <f>F3+H3</f>
         <v>3.6225628700000012</v>
       </c>
-      <c r="K3" s="1"/>
-      <c r="L3" s="3">
+      <c r="K3" s="3"/>
+      <c r="L3" s="1">
         <f>1/(1+EXP(-J3))</f>
         <v>0.97398095220758474</v>
       </c>
@@ -801,19 +803,19 @@
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="1">
         <v>5</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="1">
         <v>1.36672609</v>
       </c>
       <c r="E4" s="2"/>
       <c r="G4" s="2"/>
       <c r="I4" s="4"/>
-      <c r="K4" s="1"/>
+      <c r="K4" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>